<commit_message>
[WS2] adding new column headers to Players xl sheet
</commit_message>
<xml_diff>
--- a/Players.xlsx
+++ b/Players.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L200"/>
+  <dimension ref="A1:AF200"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -482,6 +482,106 @@
           <t>Team</t>
         </is>
       </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Matches Played</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>Matches Selected</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>Matches Started</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>Matches as a Sub</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>Captain</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>Minutes Played</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>Came On</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>Minutes as a Sub</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>Temporary Sub</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>Came Off</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>Tries</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>Drop Goals</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>Conversion Attempts</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>Conversion Scored</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>Penalties Attempts</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>Penalties Scored</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>Points</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>Sin Bin</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>Rescinded</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>Red Card</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">

</xml_diff>

<commit_message>
[DC1] adding stat heads to 'Player Stats' sheet
</commit_message>
<xml_diff>
--- a/Players.xlsx
+++ b/Players.xlsx
@@ -19904,7 +19904,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A200"/>
+  <dimension ref="A1:AC200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19918,6 +19918,146 @@
           <t>Name</t>
         </is>
       </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>MP</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>TA</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>DG</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>CA</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>MK</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>BH</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>PM</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>BTS</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>KON</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>TM</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>MT</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>DT</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>TW</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>TT</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>TC</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>HE</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>OPC</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>SPC</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>LW</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>LS</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>YC</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>RC</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">

</xml_diff>

<commit_message>
[DC2] adding new heads to 'Prediction Stats' sheet
</commit_message>
<xml_diff>
--- a/Players.xlsx
+++ b/Players.xlsx
@@ -38900,7 +38900,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC370"/>
+  <dimension ref="A1:AG370"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E25" sqref="E25"/>
@@ -39054,6 +39054,26 @@
           <t>RC</t>
         </is>
       </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>Position</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>Position No</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>Height</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>Weight</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">

</xml_diff>

<commit_message>
[DC2] adding player position column from 'Player Details' sheet to 'Prediction Stats' sheet
</commit_message>
<xml_diff>
--- a/Players.xlsx
+++ b/Players.xlsx
@@ -39165,6 +39165,11 @@
       <c r="AC2" t="n">
         <v>0</v>
       </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>Lock 5</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -39256,6 +39261,11 @@
       <c r="AC3" t="n">
         <v>0</v>
       </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>Hooker</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -39347,6 +39357,11 @@
       <c r="AC4" t="n">
         <v>0</v>
       </c>
+      <c r="AD4" t="inlineStr">
+        <is>
+          <t>Lock 4</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -39438,6 +39453,11 @@
       <c r="AC5" t="n">
         <v>0</v>
       </c>
+      <c r="AD5" t="inlineStr">
+        <is>
+          <t>Fullback</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -39529,6 +39549,11 @@
       <c r="AC6" t="n">
         <v>0</v>
       </c>
+      <c r="AD6" t="inlineStr">
+        <is>
+          <t>Lock 5</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -39620,6 +39645,11 @@
       <c r="AC7" t="n">
         <v>0</v>
       </c>
+      <c r="AD7" t="inlineStr">
+        <is>
+          <t>Lock 5</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -39711,6 +39741,11 @@
       <c r="AC8" t="n">
         <v>0</v>
       </c>
+      <c r="AD8" t="inlineStr">
+        <is>
+          <t>Loose Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -39802,6 +39837,11 @@
       <c r="AC9" t="n">
         <v>0</v>
       </c>
+      <c r="AD9" t="inlineStr">
+        <is>
+          <t>Fly Half</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -39893,6 +39933,11 @@
       <c r="AC10" t="n">
         <v>0</v>
       </c>
+      <c r="AD10" t="inlineStr">
+        <is>
+          <t>Outside Centre</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -39984,6 +40029,11 @@
       <c r="AC11" t="n">
         <v>0</v>
       </c>
+      <c r="AD11" t="inlineStr">
+        <is>
+          <t>Scrum Half</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -40075,6 +40125,11 @@
       <c r="AC12" t="n">
         <v>0</v>
       </c>
+      <c r="AD12" t="inlineStr">
+        <is>
+          <t>Fly Half</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -40166,6 +40221,11 @@
       <c r="AC13" t="n">
         <v>0</v>
       </c>
+      <c r="AD13" t="inlineStr">
+        <is>
+          <t>Tight Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -40257,6 +40317,11 @@
       <c r="AC14" t="n">
         <v>0</v>
       </c>
+      <c r="AD14" t="inlineStr">
+        <is>
+          <t>Right Wing</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -40348,6 +40413,11 @@
       <c r="AC15" t="n">
         <v>0</v>
       </c>
+      <c r="AD15" t="inlineStr">
+        <is>
+          <t>Blindside Flanker</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -40439,6 +40509,11 @@
       <c r="AC16" t="n">
         <v>0</v>
       </c>
+      <c r="AD16" t="inlineStr">
+        <is>
+          <t>Hooker</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -40530,6 +40605,11 @@
       <c r="AC17" t="n">
         <v>0</v>
       </c>
+      <c r="AD17" t="inlineStr">
+        <is>
+          <t>Lock 4</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -40621,6 +40701,11 @@
       <c r="AC18" t="n">
         <v>0</v>
       </c>
+      <c r="AD18" t="inlineStr">
+        <is>
+          <t>Loose Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -40712,6 +40797,11 @@
       <c r="AC19" t="n">
         <v>0</v>
       </c>
+      <c r="AD19" t="inlineStr">
+        <is>
+          <t>Inside Centre</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -40803,6 +40893,11 @@
       <c r="AC20" t="n">
         <v>0</v>
       </c>
+      <c r="AD20" t="inlineStr">
+        <is>
+          <t>Scrum Half</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -40894,6 +40989,11 @@
       <c r="AC21" t="n">
         <v>0</v>
       </c>
+      <c r="AD21" t="inlineStr">
+        <is>
+          <t>Left Wing</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -40985,6 +41085,11 @@
       <c r="AC22" t="n">
         <v>0</v>
       </c>
+      <c r="AD22" t="inlineStr">
+        <is>
+          <t>Fly Half</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -41076,6 +41181,11 @@
       <c r="AC23" t="n">
         <v>0</v>
       </c>
+      <c r="AD23" t="inlineStr">
+        <is>
+          <t>Outside Centre</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -41167,6 +41277,11 @@
       <c r="AC24" t="n">
         <v>0</v>
       </c>
+      <c r="AD24" t="inlineStr">
+        <is>
+          <t>Scrum Half</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -41258,6 +41373,11 @@
       <c r="AC25" t="n">
         <v>0</v>
       </c>
+      <c r="AD25" t="inlineStr">
+        <is>
+          <t>Left Wing</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -41349,6 +41469,11 @@
       <c r="AC26" t="n">
         <v>0</v>
       </c>
+      <c r="AD26" t="inlineStr">
+        <is>
+          <t>Number 8</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -41440,6 +41565,11 @@
       <c r="AC27" t="n">
         <v>0</v>
       </c>
+      <c r="AD27" t="inlineStr">
+        <is>
+          <t>Fly Half</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -41531,6 +41661,11 @@
       <c r="AC28" t="n">
         <v>0</v>
       </c>
+      <c r="AD28" t="inlineStr">
+        <is>
+          <t>Hooker</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -41622,6 +41757,11 @@
       <c r="AC29" t="n">
         <v>0</v>
       </c>
+      <c r="AD29" t="inlineStr">
+        <is>
+          <t>Right Wing</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -41713,6 +41853,11 @@
       <c r="AC30" t="n">
         <v>0</v>
       </c>
+      <c r="AD30" t="inlineStr">
+        <is>
+          <t>Openside Flanker</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -41804,6 +41949,11 @@
       <c r="AC31" t="n">
         <v>0</v>
       </c>
+      <c r="AD31" t="inlineStr">
+        <is>
+          <t>Fly Half</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -41895,6 +42045,11 @@
       <c r="AC32" t="n">
         <v>0</v>
       </c>
+      <c r="AD32" t="inlineStr">
+        <is>
+          <t>Tight Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -41986,6 +42141,11 @@
       <c r="AC33" t="n">
         <v>0</v>
       </c>
+      <c r="AD33" t="inlineStr">
+        <is>
+          <t>Scrum Half</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -42077,6 +42237,11 @@
       <c r="AC34" t="n">
         <v>0</v>
       </c>
+      <c r="AD34" t="inlineStr">
+        <is>
+          <t>Openside Flanker</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -42168,6 +42333,11 @@
       <c r="AC35" t="n">
         <v>0</v>
       </c>
+      <c r="AD35" t="inlineStr">
+        <is>
+          <t>Outside Centre</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -42259,6 +42429,11 @@
       <c r="AC36" t="n">
         <v>0</v>
       </c>
+      <c r="AD36" t="inlineStr">
+        <is>
+          <t>Scrum Half</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -42350,6 +42525,11 @@
       <c r="AC37" t="n">
         <v>0</v>
       </c>
+      <c r="AD37" t="inlineStr">
+        <is>
+          <t>Hooker</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -42441,6 +42621,11 @@
       <c r="AC38" t="n">
         <v>0</v>
       </c>
+      <c r="AD38" t="inlineStr">
+        <is>
+          <t>Scrum Half</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -42532,6 +42717,11 @@
       <c r="AC39" t="n">
         <v>0</v>
       </c>
+      <c r="AD39" t="inlineStr">
+        <is>
+          <t>Outside Centre</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -42623,6 +42813,11 @@
       <c r="AC40" t="n">
         <v>0</v>
       </c>
+      <c r="AD40" t="inlineStr">
+        <is>
+          <t>Fullback</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -42714,6 +42909,11 @@
       <c r="AC41" t="n">
         <v>0</v>
       </c>
+      <c r="AD41" t="inlineStr">
+        <is>
+          <t>Number 8</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -42805,6 +43005,11 @@
       <c r="AC42" t="n">
         <v>0</v>
       </c>
+      <c r="AD42" t="inlineStr">
+        <is>
+          <t>Lock 5</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -42896,6 +43101,11 @@
       <c r="AC43" t="n">
         <v>0</v>
       </c>
+      <c r="AD43" t="inlineStr">
+        <is>
+          <t>Openside Flanker</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -42987,6 +43197,11 @@
       <c r="AC44" t="n">
         <v>0</v>
       </c>
+      <c r="AD44" t="inlineStr">
+        <is>
+          <t>Tight Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -43078,6 +43293,11 @@
       <c r="AC45" t="n">
         <v>0</v>
       </c>
+      <c r="AD45" t="inlineStr">
+        <is>
+          <t>Loose Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -43169,6 +43389,11 @@
       <c r="AC46" t="n">
         <v>0</v>
       </c>
+      <c r="AD46" t="inlineStr">
+        <is>
+          <t>Tight Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -43260,6 +43485,11 @@
       <c r="AC47" t="n">
         <v>0</v>
       </c>
+      <c r="AD47" t="inlineStr">
+        <is>
+          <t>Hooker</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -43351,6 +43581,11 @@
       <c r="AC48" t="n">
         <v>0</v>
       </c>
+      <c r="AD48" t="inlineStr">
+        <is>
+          <t>Hooker</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -43442,6 +43677,11 @@
       <c r="AC49" t="n">
         <v>0</v>
       </c>
+      <c r="AD49" t="inlineStr">
+        <is>
+          <t>Hooker</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -43533,6 +43773,11 @@
       <c r="AC50" t="n">
         <v>0</v>
       </c>
+      <c r="AD50" t="inlineStr">
+        <is>
+          <t>Lock 5</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -43624,6 +43869,11 @@
       <c r="AC51" t="n">
         <v>0</v>
       </c>
+      <c r="AD51" t="inlineStr">
+        <is>
+          <t>Blindside Flanker</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -43715,6 +43965,11 @@
       <c r="AC52" t="n">
         <v>0</v>
       </c>
+      <c r="AD52" t="inlineStr">
+        <is>
+          <t>Tight Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -43806,6 +44061,11 @@
       <c r="AC53" t="n">
         <v>0</v>
       </c>
+      <c r="AD53" t="inlineStr">
+        <is>
+          <t>Left Wing</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -43897,6 +44157,11 @@
       <c r="AC54" t="n">
         <v>0</v>
       </c>
+      <c r="AD54" t="inlineStr">
+        <is>
+          <t>Fly Half</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -43988,6 +44253,11 @@
       <c r="AC55" t="n">
         <v>0</v>
       </c>
+      <c r="AD55" t="inlineStr">
+        <is>
+          <t>Scrum Half</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -44079,6 +44349,11 @@
       <c r="AC56" t="n">
         <v>0</v>
       </c>
+      <c r="AD56" t="inlineStr">
+        <is>
+          <t>Openside Flanker</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -44170,6 +44445,11 @@
       <c r="AC57" t="n">
         <v>0</v>
       </c>
+      <c r="AD57" t="inlineStr">
+        <is>
+          <t>Lock 5</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -44261,6 +44541,11 @@
       <c r="AC58" t="n">
         <v>0</v>
       </c>
+      <c r="AD58" t="inlineStr">
+        <is>
+          <t>Scrum Half</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -44352,6 +44637,11 @@
       <c r="AC59" t="n">
         <v>0</v>
       </c>
+      <c r="AD59" t="inlineStr">
+        <is>
+          <t>Outside Centre</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -44443,6 +44733,11 @@
       <c r="AC60" t="n">
         <v>0</v>
       </c>
+      <c r="AD60" t="inlineStr">
+        <is>
+          <t>Right Wing</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -44534,6 +44829,11 @@
       <c r="AC61" t="n">
         <v>0</v>
       </c>
+      <c r="AD61" t="inlineStr">
+        <is>
+          <t>Fly Half</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -44625,6 +44925,11 @@
       <c r="AC62" t="n">
         <v>0</v>
       </c>
+      <c r="AD62" t="inlineStr">
+        <is>
+          <t>Fullback</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -44716,6 +45021,11 @@
       <c r="AC63" t="n">
         <v>0</v>
       </c>
+      <c r="AD63" t="inlineStr">
+        <is>
+          <t>Left Wing</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -44807,6 +45117,11 @@
       <c r="AC64" t="n">
         <v>0</v>
       </c>
+      <c r="AD64" t="inlineStr">
+        <is>
+          <t>Tight Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -44898,6 +45213,11 @@
       <c r="AC65" t="n">
         <v>0</v>
       </c>
+      <c r="AD65" t="inlineStr">
+        <is>
+          <t>Left Wing</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -44989,6 +45309,11 @@
       <c r="AC66" t="n">
         <v>0</v>
       </c>
+      <c r="AD66" t="inlineStr">
+        <is>
+          <t>Lock 4</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -45080,6 +45405,11 @@
       <c r="AC67" t="n">
         <v>0</v>
       </c>
+      <c r="AD67" t="inlineStr">
+        <is>
+          <t>Lock 5</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -45171,6 +45501,11 @@
       <c r="AC68" t="n">
         <v>0</v>
       </c>
+      <c r="AD68" t="inlineStr">
+        <is>
+          <t>Openside Flanker</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -45262,6 +45597,11 @@
       <c r="AC69" t="n">
         <v>0</v>
       </c>
+      <c r="AD69" t="inlineStr">
+        <is>
+          <t>Lock 4</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -45353,6 +45693,11 @@
       <c r="AC70" t="n">
         <v>0</v>
       </c>
+      <c r="AD70" t="inlineStr">
+        <is>
+          <t>Openside Flanker</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -45444,6 +45789,11 @@
       <c r="AC71" t="n">
         <v>0</v>
       </c>
+      <c r="AD71" t="inlineStr">
+        <is>
+          <t>Blindside Flanker</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -45535,6 +45885,11 @@
       <c r="AC72" t="n">
         <v>0</v>
       </c>
+      <c r="AD72" t="inlineStr">
+        <is>
+          <t>Loose Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -45626,6 +45981,11 @@
       <c r="AC73" t="n">
         <v>0</v>
       </c>
+      <c r="AD73" t="inlineStr">
+        <is>
+          <t>Loose Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -45717,6 +46077,11 @@
       <c r="AC74" t="n">
         <v>0</v>
       </c>
+      <c r="AD74" t="inlineStr">
+        <is>
+          <t>Inside Centre</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -45808,6 +46173,11 @@
       <c r="AC75" t="n">
         <v>0</v>
       </c>
+      <c r="AD75" t="inlineStr">
+        <is>
+          <t>Tight Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -45899,6 +46269,11 @@
       <c r="AC76" t="n">
         <v>0</v>
       </c>
+      <c r="AD76" t="inlineStr">
+        <is>
+          <t>Inside Centre</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -45990,6 +46365,11 @@
       <c r="AC77" t="n">
         <v>0</v>
       </c>
+      <c r="AD77" t="inlineStr">
+        <is>
+          <t>Lock 5</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -46081,6 +46461,11 @@
       <c r="AC78" t="n">
         <v>0</v>
       </c>
+      <c r="AD78" t="inlineStr">
+        <is>
+          <t>Outside Centre</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -46172,6 +46557,11 @@
       <c r="AC79" t="n">
         <v>0</v>
       </c>
+      <c r="AD79" t="inlineStr">
+        <is>
+          <t>Fly Half</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -46263,6 +46653,11 @@
       <c r="AC80" t="n">
         <v>0</v>
       </c>
+      <c r="AD80" t="inlineStr">
+        <is>
+          <t>Lock 4</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -46354,6 +46749,11 @@
       <c r="AC81" t="n">
         <v>0</v>
       </c>
+      <c r="AD81" t="inlineStr">
+        <is>
+          <t>Outside Centre</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -46445,6 +46845,11 @@
       <c r="AC82" t="n">
         <v>0</v>
       </c>
+      <c r="AD82" t="inlineStr">
+        <is>
+          <t>Loose Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -46536,6 +46941,11 @@
       <c r="AC83" t="n">
         <v>0</v>
       </c>
+      <c r="AD83" t="inlineStr">
+        <is>
+          <t>Left Wing</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -46627,6 +47037,11 @@
       <c r="AC84" t="n">
         <v>0</v>
       </c>
+      <c r="AD84" t="inlineStr">
+        <is>
+          <t>Openside Flanker</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -46718,6 +47133,11 @@
       <c r="AC85" t="n">
         <v>0</v>
       </c>
+      <c r="AD85" t="inlineStr">
+        <is>
+          <t>Tight Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -46809,6 +47229,11 @@
       <c r="AC86" t="n">
         <v>0</v>
       </c>
+      <c r="AD86" t="inlineStr">
+        <is>
+          <t>Blindside Flanker</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -46900,6 +47325,11 @@
       <c r="AC87" t="n">
         <v>0</v>
       </c>
+      <c r="AD87" t="inlineStr">
+        <is>
+          <t>Loose Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -46991,6 +47421,11 @@
       <c r="AC88" t="n">
         <v>0</v>
       </c>
+      <c r="AD88" t="inlineStr">
+        <is>
+          <t>Inside Centre</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -47082,6 +47517,11 @@
       <c r="AC89" t="n">
         <v>0</v>
       </c>
+      <c r="AD89" t="inlineStr">
+        <is>
+          <t>Lock 5</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -47173,6 +47613,11 @@
       <c r="AC90" t="n">
         <v>0</v>
       </c>
+      <c r="AD90" t="inlineStr">
+        <is>
+          <t>Loose Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -47264,6 +47709,11 @@
       <c r="AC91" t="n">
         <v>0</v>
       </c>
+      <c r="AD91" t="inlineStr">
+        <is>
+          <t>Openside Flanker</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -47355,6 +47805,11 @@
       <c r="AC92" t="n">
         <v>0</v>
       </c>
+      <c r="AD92" t="inlineStr">
+        <is>
+          <t>Outside Centre</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -47446,6 +47901,11 @@
       <c r="AC93" t="n">
         <v>0</v>
       </c>
+      <c r="AD93" t="inlineStr">
+        <is>
+          <t>Fullback</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -47537,6 +47997,11 @@
       <c r="AC94" t="n">
         <v>0</v>
       </c>
+      <c r="AD94" t="inlineStr">
+        <is>
+          <t>Inside Centre</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -47628,6 +48093,11 @@
       <c r="AC95" t="n">
         <v>0</v>
       </c>
+      <c r="AD95" t="inlineStr">
+        <is>
+          <t>Hooker</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -47719,6 +48189,11 @@
       <c r="AC96" t="n">
         <v>0</v>
       </c>
+      <c r="AD96" t="inlineStr">
+        <is>
+          <t>Lock 4</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -47810,6 +48285,11 @@
       <c r="AC97" t="n">
         <v>0</v>
       </c>
+      <c r="AD97" t="inlineStr">
+        <is>
+          <t>Number 8</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -47901,6 +48381,11 @@
       <c r="AC98" t="n">
         <v>0</v>
       </c>
+      <c r="AD98" t="inlineStr">
+        <is>
+          <t>Openside Flanker</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -47992,6 +48477,11 @@
       <c r="AC99" t="n">
         <v>0</v>
       </c>
+      <c r="AD99" t="inlineStr">
+        <is>
+          <t>Fly Half</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -48083,6 +48573,11 @@
       <c r="AC100" t="n">
         <v>0</v>
       </c>
+      <c r="AD100" t="inlineStr">
+        <is>
+          <t>Lock 5</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -48174,6 +48669,11 @@
       <c r="AC101" t="n">
         <v>0</v>
       </c>
+      <c r="AD101" t="inlineStr">
+        <is>
+          <t>Blindside Flanker</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -48265,6 +48765,11 @@
       <c r="AC102" t="n">
         <v>0</v>
       </c>
+      <c r="AD102" t="inlineStr">
+        <is>
+          <t>Right Wing</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -48356,6 +48861,11 @@
       <c r="AC103" t="n">
         <v>0</v>
       </c>
+      <c r="AD103" t="inlineStr">
+        <is>
+          <t>Number 8</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -48447,6 +48957,11 @@
       <c r="AC104" t="n">
         <v>0</v>
       </c>
+      <c r="AD104" t="inlineStr">
+        <is>
+          <t>Loose Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -48538,6 +49053,11 @@
       <c r="AC105" t="n">
         <v>0</v>
       </c>
+      <c r="AD105" t="inlineStr">
+        <is>
+          <t>Tight Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -48629,6 +49149,11 @@
       <c r="AC106" t="n">
         <v>0</v>
       </c>
+      <c r="AD106" t="inlineStr">
+        <is>
+          <t>Inside Centre</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -48720,6 +49245,11 @@
       <c r="AC107" t="n">
         <v>0</v>
       </c>
+      <c r="AD107" t="inlineStr">
+        <is>
+          <t>Hooker</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -48811,6 +49341,11 @@
       <c r="AC108" t="n">
         <v>0</v>
       </c>
+      <c r="AD108" t="inlineStr">
+        <is>
+          <t>Lock 5</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -48902,6 +49437,11 @@
       <c r="AC109" t="n">
         <v>0</v>
       </c>
+      <c r="AD109" t="inlineStr">
+        <is>
+          <t>Hooker</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -48993,6 +49533,11 @@
       <c r="AC110" t="n">
         <v>0</v>
       </c>
+      <c r="AD110" t="inlineStr">
+        <is>
+          <t>Lock 4</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -49084,6 +49629,11 @@
       <c r="AC111" t="n">
         <v>0</v>
       </c>
+      <c r="AD111" t="inlineStr">
+        <is>
+          <t>Fullback</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -49175,6 +49725,11 @@
       <c r="AC112" t="n">
         <v>0</v>
       </c>
+      <c r="AD112" t="inlineStr">
+        <is>
+          <t>Lock 5</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -49266,6 +49821,11 @@
       <c r="AC113" t="n">
         <v>0</v>
       </c>
+      <c r="AD113" t="inlineStr">
+        <is>
+          <t>Lock 5</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -49357,6 +49917,11 @@
       <c r="AC114" t="n">
         <v>0</v>
       </c>
+      <c r="AD114" t="inlineStr">
+        <is>
+          <t>Loose Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -49448,6 +50013,11 @@
       <c r="AC115" t="n">
         <v>0</v>
       </c>
+      <c r="AD115" t="inlineStr">
+        <is>
+          <t>Scrum Half</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -49539,6 +50109,11 @@
       <c r="AC116" t="n">
         <v>0</v>
       </c>
+      <c r="AD116" t="inlineStr">
+        <is>
+          <t>Fly Half</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -49630,6 +50205,11 @@
       <c r="AC117" t="n">
         <v>0</v>
       </c>
+      <c r="AD117" t="inlineStr">
+        <is>
+          <t>Outside Centre</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -49721,6 +50301,11 @@
       <c r="AC118" t="n">
         <v>0</v>
       </c>
+      <c r="AD118" t="inlineStr">
+        <is>
+          <t>Scrum Half</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -49812,6 +50397,11 @@
       <c r="AC119" t="n">
         <v>0</v>
       </c>
+      <c r="AD119" t="inlineStr">
+        <is>
+          <t>Inside Centre</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -49903,6 +50493,11 @@
       <c r="AC120" t="n">
         <v>0</v>
       </c>
+      <c r="AD120" t="inlineStr">
+        <is>
+          <t>Fly Half</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -49994,6 +50589,11 @@
       <c r="AC121" t="n">
         <v>0</v>
       </c>
+      <c r="AD121" t="inlineStr">
+        <is>
+          <t>Fly Half</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -50085,6 +50685,11 @@
       <c r="AC122" t="n">
         <v>0</v>
       </c>
+      <c r="AD122" t="inlineStr">
+        <is>
+          <t>Tight Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -50176,6 +50781,11 @@
       <c r="AC123" t="n">
         <v>0</v>
       </c>
+      <c r="AD123" t="inlineStr">
+        <is>
+          <t>Right Wing</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -50267,6 +50877,11 @@
       <c r="AC124" t="n">
         <v>0</v>
       </c>
+      <c r="AD124" t="inlineStr">
+        <is>
+          <t>Blindside Flanker</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -50358,6 +50973,11 @@
       <c r="AC125" t="n">
         <v>0</v>
       </c>
+      <c r="AD125" t="inlineStr">
+        <is>
+          <t>Hooker</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -50449,6 +51069,11 @@
       <c r="AC126" t="n">
         <v>0</v>
       </c>
+      <c r="AD126" t="inlineStr">
+        <is>
+          <t>Lock 4</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -50540,6 +51165,11 @@
       <c r="AC127" t="n">
         <v>0</v>
       </c>
+      <c r="AD127" t="inlineStr">
+        <is>
+          <t>Loose Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -50631,6 +51261,11 @@
       <c r="AC128" t="n">
         <v>0</v>
       </c>
+      <c r="AD128" t="inlineStr">
+        <is>
+          <t>Inside Centre</t>
+        </is>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -50722,6 +51357,11 @@
       <c r="AC129" t="n">
         <v>0</v>
       </c>
+      <c r="AD129" t="inlineStr">
+        <is>
+          <t>Number 8</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -50813,6 +51453,11 @@
       <c r="AC130" t="n">
         <v>0</v>
       </c>
+      <c r="AD130" t="inlineStr">
+        <is>
+          <t>Scrum Half</t>
+        </is>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -50904,6 +51549,11 @@
       <c r="AC131" t="n">
         <v>0</v>
       </c>
+      <c r="AD131" t="inlineStr">
+        <is>
+          <t>Left Wing</t>
+        </is>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -50995,6 +51645,11 @@
       <c r="AC132" t="n">
         <v>0</v>
       </c>
+      <c r="AD132" t="inlineStr">
+        <is>
+          <t>Fly Half</t>
+        </is>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -51086,6 +51741,11 @@
       <c r="AC133" t="n">
         <v>0</v>
       </c>
+      <c r="AD133" t="inlineStr">
+        <is>
+          <t>Inside Centre</t>
+        </is>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -51177,6 +51837,11 @@
       <c r="AC134" t="n">
         <v>0</v>
       </c>
+      <c r="AD134" t="inlineStr">
+        <is>
+          <t>Outside Centre</t>
+        </is>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -51268,6 +51933,11 @@
       <c r="AC135" t="n">
         <v>0</v>
       </c>
+      <c r="AD135" t="inlineStr">
+        <is>
+          <t>Loose Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -51359,6 +52029,11 @@
       <c r="AC136" t="n">
         <v>0</v>
       </c>
+      <c r="AD136" t="inlineStr">
+        <is>
+          <t>Scrum Half</t>
+        </is>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -51450,6 +52125,11 @@
       <c r="AC137" t="n">
         <v>0</v>
       </c>
+      <c r="AD137" t="inlineStr">
+        <is>
+          <t>Left Wing</t>
+        </is>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -51541,6 +52221,11 @@
       <c r="AC138" t="n">
         <v>0</v>
       </c>
+      <c r="AD138" t="inlineStr">
+        <is>
+          <t>Fullback</t>
+        </is>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -51632,6 +52317,11 @@
       <c r="AC139" t="n">
         <v>0</v>
       </c>
+      <c r="AD139" t="inlineStr">
+        <is>
+          <t>Number 8</t>
+        </is>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -51723,6 +52413,11 @@
       <c r="AC140" t="n">
         <v>0</v>
       </c>
+      <c r="AD140" t="inlineStr">
+        <is>
+          <t>Right Wing</t>
+        </is>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -51814,6 +52509,11 @@
       <c r="AC141" t="n">
         <v>0</v>
       </c>
+      <c r="AD141" t="inlineStr">
+        <is>
+          <t>Fly Half</t>
+        </is>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -51905,6 +52605,11 @@
       <c r="AC142" t="n">
         <v>0</v>
       </c>
+      <c r="AD142" t="inlineStr">
+        <is>
+          <t>Blindside Flanker</t>
+        </is>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -51996,6 +52701,11 @@
       <c r="AC143" t="n">
         <v>0</v>
       </c>
+      <c r="AD143" t="inlineStr">
+        <is>
+          <t>Hooker</t>
+        </is>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -52087,6 +52797,11 @@
       <c r="AC144" t="n">
         <v>0</v>
       </c>
+      <c r="AD144" t="inlineStr">
+        <is>
+          <t>Right Wing</t>
+        </is>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -52178,6 +52893,11 @@
       <c r="AC145" t="n">
         <v>0</v>
       </c>
+      <c r="AD145" t="inlineStr">
+        <is>
+          <t>Openside Flanker</t>
+        </is>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -52269,6 +52989,11 @@
       <c r="AC146" t="n">
         <v>0</v>
       </c>
+      <c r="AD146" t="inlineStr">
+        <is>
+          <t>Fly Half</t>
+        </is>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -52360,6 +53085,11 @@
       <c r="AC147" t="n">
         <v>0</v>
       </c>
+      <c r="AD147" t="inlineStr">
+        <is>
+          <t>Hooker</t>
+        </is>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -52451,6 +53181,11 @@
       <c r="AC148" t="n">
         <v>0</v>
       </c>
+      <c r="AD148" t="inlineStr">
+        <is>
+          <t>Tight Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -52542,6 +53277,11 @@
       <c r="AC149" t="n">
         <v>0</v>
       </c>
+      <c r="AD149" t="inlineStr">
+        <is>
+          <t>Scrum Half</t>
+        </is>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -52633,6 +53373,11 @@
       <c r="AC150" t="n">
         <v>0</v>
       </c>
+      <c r="AD150" t="inlineStr">
+        <is>
+          <t>Tight Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -52724,6 +53469,11 @@
       <c r="AC151" t="n">
         <v>0</v>
       </c>
+      <c r="AD151" t="inlineStr">
+        <is>
+          <t>Openside Flanker</t>
+        </is>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -52815,6 +53565,11 @@
       <c r="AC152" t="n">
         <v>0</v>
       </c>
+      <c r="AD152" t="inlineStr">
+        <is>
+          <t>Outside Centre</t>
+        </is>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -52906,6 +53661,11 @@
       <c r="AC153" t="n">
         <v>0</v>
       </c>
+      <c r="AD153" t="inlineStr">
+        <is>
+          <t>Left Wing</t>
+        </is>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -52997,6 +53757,11 @@
       <c r="AC154" t="n">
         <v>0</v>
       </c>
+      <c r="AD154" t="inlineStr">
+        <is>
+          <t>Blindside Flanker</t>
+        </is>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -53088,6 +53853,11 @@
       <c r="AC155" t="n">
         <v>0</v>
       </c>
+      <c r="AD155" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -53179,6 +53949,11 @@
       <c r="AC156" t="n">
         <v>0</v>
       </c>
+      <c r="AD156" t="inlineStr">
+        <is>
+          <t>Scrum Half</t>
+        </is>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -53270,6 +54045,11 @@
       <c r="AC157" t="n">
         <v>0</v>
       </c>
+      <c r="AD157" t="inlineStr">
+        <is>
+          <t>Hooker</t>
+        </is>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -53361,6 +54141,11 @@
       <c r="AC158" t="n">
         <v>0</v>
       </c>
+      <c r="AD158" t="inlineStr">
+        <is>
+          <t>Scrum Half</t>
+        </is>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -53452,6 +54237,11 @@
       <c r="AC159" t="n">
         <v>0</v>
       </c>
+      <c r="AD159" t="inlineStr">
+        <is>
+          <t>Scrum Half</t>
+        </is>
+      </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -53543,6 +54333,11 @@
       <c r="AC160" t="n">
         <v>0</v>
       </c>
+      <c r="AD160" t="inlineStr">
+        <is>
+          <t>Outside Centre</t>
+        </is>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -53634,6 +54429,11 @@
       <c r="AC161" t="n">
         <v>0</v>
       </c>
+      <c r="AD161" t="inlineStr">
+        <is>
+          <t>Openside Flanker</t>
+        </is>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -53725,6 +54525,11 @@
       <c r="AC162" t="n">
         <v>0</v>
       </c>
+      <c r="AD162" t="inlineStr">
+        <is>
+          <t>Fullback</t>
+        </is>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -53816,6 +54621,11 @@
       <c r="AC163" t="n">
         <v>0</v>
       </c>
+      <c r="AD163" t="inlineStr">
+        <is>
+          <t>Loose Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -53907,6 +54717,11 @@
       <c r="AC164" t="n">
         <v>0</v>
       </c>
+      <c r="AD164" t="inlineStr">
+        <is>
+          <t>Lock 5</t>
+        </is>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -53998,6 +54813,11 @@
       <c r="AC165" t="n">
         <v>0</v>
       </c>
+      <c r="AD165" t="inlineStr">
+        <is>
+          <t>Fullback</t>
+        </is>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -54089,6 +54909,11 @@
       <c r="AC166" t="n">
         <v>0</v>
       </c>
+      <c r="AD166" t="inlineStr">
+        <is>
+          <t>Openside Flanker</t>
+        </is>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -54180,6 +55005,11 @@
       <c r="AC167" t="n">
         <v>0</v>
       </c>
+      <c r="AD167" t="inlineStr">
+        <is>
+          <t>Blindside Flanker</t>
+        </is>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -54271,6 +55101,11 @@
       <c r="AC168" t="n">
         <v>0</v>
       </c>
+      <c r="AD168" t="inlineStr">
+        <is>
+          <t>Tight Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -54362,6 +55197,11 @@
       <c r="AC169" t="n">
         <v>0</v>
       </c>
+      <c r="AD169" t="inlineStr">
+        <is>
+          <t>Loose Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -54453,6 +55293,11 @@
       <c r="AC170" t="n">
         <v>0</v>
       </c>
+      <c r="AD170" t="inlineStr">
+        <is>
+          <t>Hooker</t>
+        </is>
+      </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -54544,6 +55389,11 @@
       <c r="AC171" t="n">
         <v>0</v>
       </c>
+      <c r="AD171" t="inlineStr">
+        <is>
+          <t>Scrum Half</t>
+        </is>
+      </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -54635,6 +55485,11 @@
       <c r="AC172" t="n">
         <v>0</v>
       </c>
+      <c r="AD172" t="inlineStr">
+        <is>
+          <t>Hooker</t>
+        </is>
+      </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -54726,6 +55581,11 @@
       <c r="AC173" t="n">
         <v>0</v>
       </c>
+      <c r="AD173" t="inlineStr">
+        <is>
+          <t>Lock 4</t>
+        </is>
+      </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -54817,6 +55677,11 @@
       <c r="AC174" t="n">
         <v>0</v>
       </c>
+      <c r="AD174" t="inlineStr">
+        <is>
+          <t>Scrum Half</t>
+        </is>
+      </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -54908,6 +55773,11 @@
       <c r="AC175" t="n">
         <v>0</v>
       </c>
+      <c r="AD175" t="inlineStr">
+        <is>
+          <t>Hooker</t>
+        </is>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -54999,6 +55869,11 @@
       <c r="AC176" t="n">
         <v>0</v>
       </c>
+      <c r="AD176" t="inlineStr">
+        <is>
+          <t>Hooker</t>
+        </is>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -55090,6 +55965,11 @@
       <c r="AC177" t="n">
         <v>0</v>
       </c>
+      <c r="AD177" t="inlineStr">
+        <is>
+          <t>Lock 5</t>
+        </is>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -55181,6 +56061,11 @@
       <c r="AC178" t="n">
         <v>0</v>
       </c>
+      <c r="AD178" t="inlineStr">
+        <is>
+          <t>Blindside Flanker</t>
+        </is>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -55272,6 +56157,11 @@
       <c r="AC179" t="n">
         <v>0</v>
       </c>
+      <c r="AD179" t="inlineStr">
+        <is>
+          <t>Left Wing</t>
+        </is>
+      </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -55363,6 +56253,11 @@
       <c r="AC180" t="n">
         <v>0</v>
       </c>
+      <c r="AD180" t="inlineStr">
+        <is>
+          <t>Left Wing</t>
+        </is>
+      </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -55454,6 +56349,11 @@
       <c r="AC181" t="n">
         <v>0</v>
       </c>
+      <c r="AD181" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -55545,6 +56445,11 @@
       <c r="AC182" t="n">
         <v>0</v>
       </c>
+      <c r="AD182" t="inlineStr">
+        <is>
+          <t>Openside Flanker</t>
+        </is>
+      </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -55636,6 +56541,11 @@
       <c r="AC183" t="n">
         <v>0</v>
       </c>
+      <c r="AD183" t="inlineStr">
+        <is>
+          <t>Lock 5</t>
+        </is>
+      </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -55727,6 +56637,11 @@
       <c r="AC184" t="n">
         <v>0</v>
       </c>
+      <c r="AD184" t="inlineStr">
+        <is>
+          <t>Scrum Half</t>
+        </is>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -55818,6 +56733,11 @@
       <c r="AC185" t="n">
         <v>0</v>
       </c>
+      <c r="AD185" t="inlineStr">
+        <is>
+          <t>Outside Centre</t>
+        </is>
+      </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -55909,6 +56829,11 @@
       <c r="AC186" t="n">
         <v>0</v>
       </c>
+      <c r="AD186" t="inlineStr">
+        <is>
+          <t>Fullback</t>
+        </is>
+      </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -56000,6 +56925,11 @@
       <c r="AC187" t="n">
         <v>0</v>
       </c>
+      <c r="AD187" t="inlineStr">
+        <is>
+          <t>Right Wing</t>
+        </is>
+      </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -56091,6 +57021,11 @@
       <c r="AC188" t="n">
         <v>0</v>
       </c>
+      <c r="AD188" t="inlineStr">
+        <is>
+          <t>Fly Half</t>
+        </is>
+      </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -56182,6 +57117,11 @@
       <c r="AC189" t="n">
         <v>0</v>
       </c>
+      <c r="AD189" t="inlineStr">
+        <is>
+          <t>Fullback</t>
+        </is>
+      </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -56273,6 +57213,11 @@
       <c r="AC190" t="n">
         <v>0</v>
       </c>
+      <c r="AD190" t="inlineStr">
+        <is>
+          <t>Left Wing</t>
+        </is>
+      </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -56364,6 +57309,11 @@
       <c r="AC191" t="n">
         <v>0</v>
       </c>
+      <c r="AD191" t="inlineStr">
+        <is>
+          <t>Lock 4</t>
+        </is>
+      </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -56455,6 +57405,11 @@
       <c r="AC192" t="n">
         <v>0</v>
       </c>
+      <c r="AD192" t="inlineStr">
+        <is>
+          <t>Tight Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
@@ -56546,6 +57501,11 @@
       <c r="AC193" t="n">
         <v>0</v>
       </c>
+      <c r="AD193" t="inlineStr">
+        <is>
+          <t>Hooker</t>
+        </is>
+      </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -56637,6 +57597,11 @@
       <c r="AC194" t="n">
         <v>0</v>
       </c>
+      <c r="AD194" t="inlineStr">
+        <is>
+          <t>Left Wing</t>
+        </is>
+      </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -56728,6 +57693,11 @@
       <c r="AC195" t="n">
         <v>0</v>
       </c>
+      <c r="AD195" t="inlineStr">
+        <is>
+          <t>Lock 4</t>
+        </is>
+      </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -56819,6 +57789,11 @@
       <c r="AC196" t="n">
         <v>0</v>
       </c>
+      <c r="AD196" t="inlineStr">
+        <is>
+          <t>Lock 5</t>
+        </is>
+      </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -56910,6 +57885,11 @@
       <c r="AC197" t="n">
         <v>0</v>
       </c>
+      <c r="AD197" t="inlineStr">
+        <is>
+          <t>Loose Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
@@ -57001,6 +57981,11 @@
       <c r="AC198" t="n">
         <v>0</v>
       </c>
+      <c r="AD198" t="inlineStr">
+        <is>
+          <t>Openside Flanker</t>
+        </is>
+      </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
@@ -57092,6 +58077,11 @@
       <c r="AC199" t="n">
         <v>0</v>
       </c>
+      <c r="AD199" t="inlineStr">
+        <is>
+          <t>Openside Flanker</t>
+        </is>
+      </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
@@ -57183,6 +58173,11 @@
       <c r="AC200" t="n">
         <v>0</v>
       </c>
+      <c r="AD200" t="inlineStr">
+        <is>
+          <t>Fly Half</t>
+        </is>
+      </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
@@ -57274,6 +58269,11 @@
       <c r="AC201" t="n">
         <v>0</v>
       </c>
+      <c r="AD201" t="inlineStr">
+        <is>
+          <t>Blindside Flanker</t>
+        </is>
+      </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
@@ -57365,6 +58365,11 @@
       <c r="AC202" t="n">
         <v>0</v>
       </c>
+      <c r="AD202" t="inlineStr">
+        <is>
+          <t>Loose Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
@@ -57456,6 +58461,11 @@
       <c r="AC203" t="n">
         <v>0</v>
       </c>
+      <c r="AD203" t="inlineStr">
+        <is>
+          <t>Loose Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
@@ -57547,6 +58557,11 @@
       <c r="AC204" t="n">
         <v>0</v>
       </c>
+      <c r="AD204" t="inlineStr">
+        <is>
+          <t>Loose Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
@@ -57638,6 +58653,11 @@
       <c r="AC205" t="n">
         <v>0</v>
       </c>
+      <c r="AD205" t="inlineStr">
+        <is>
+          <t>Outside Centre</t>
+        </is>
+      </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
@@ -57729,6 +58749,11 @@
       <c r="AC206" t="n">
         <v>0</v>
       </c>
+      <c r="AD206" t="inlineStr">
+        <is>
+          <t>Blindside Flanker</t>
+        </is>
+      </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
@@ -57820,6 +58845,11 @@
       <c r="AC207" t="n">
         <v>0</v>
       </c>
+      <c r="AD207" t="inlineStr">
+        <is>
+          <t>Tight Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
@@ -57911,6 +58941,11 @@
       <c r="AC208" t="n">
         <v>0</v>
       </c>
+      <c r="AD208" t="inlineStr">
+        <is>
+          <t>Loose Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
@@ -58002,6 +59037,11 @@
       <c r="AC209" t="n">
         <v>0</v>
       </c>
+      <c r="AD209" t="inlineStr">
+        <is>
+          <t>Inside Centre</t>
+        </is>
+      </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
@@ -58093,6 +59133,11 @@
       <c r="AC210" t="n">
         <v>0</v>
       </c>
+      <c r="AD210" t="inlineStr">
+        <is>
+          <t>Tight Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
@@ -58184,6 +59229,11 @@
       <c r="AC211" t="n">
         <v>0</v>
       </c>
+      <c r="AD211" t="inlineStr">
+        <is>
+          <t>Inside Centre</t>
+        </is>
+      </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
@@ -58275,6 +59325,11 @@
       <c r="AC212" t="n">
         <v>0</v>
       </c>
+      <c r="AD212" t="inlineStr">
+        <is>
+          <t>Left Wing</t>
+        </is>
+      </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
@@ -58366,6 +59421,11 @@
       <c r="AC213" t="n">
         <v>0</v>
       </c>
+      <c r="AD213" t="inlineStr">
+        <is>
+          <t>Lock 5</t>
+        </is>
+      </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
@@ -58457,6 +59517,11 @@
       <c r="AC214" t="n">
         <v>0</v>
       </c>
+      <c r="AD214" t="inlineStr">
+        <is>
+          <t>Outside Centre</t>
+        </is>
+      </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
@@ -58548,6 +59613,11 @@
       <c r="AC215" t="n">
         <v>0</v>
       </c>
+      <c r="AD215" t="inlineStr">
+        <is>
+          <t>Tight Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
@@ -58639,6 +59709,11 @@
       <c r="AC216" t="n">
         <v>0</v>
       </c>
+      <c r="AD216" t="inlineStr">
+        <is>
+          <t>Fly Half</t>
+        </is>
+      </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
@@ -58730,6 +59805,11 @@
       <c r="AC217" t="n">
         <v>0</v>
       </c>
+      <c r="AD217" t="inlineStr">
+        <is>
+          <t>Lock 4</t>
+        </is>
+      </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
@@ -58821,6 +59901,11 @@
       <c r="AC218" t="n">
         <v>0</v>
       </c>
+      <c r="AD218" t="inlineStr">
+        <is>
+          <t>Hooker</t>
+        </is>
+      </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
@@ -58912,6 +59997,11 @@
       <c r="AC219" t="n">
         <v>0</v>
       </c>
+      <c r="AD219" t="inlineStr">
+        <is>
+          <t>Tight Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
@@ -59003,6 +60093,11 @@
       <c r="AC220" t="n">
         <v>1</v>
       </c>
+      <c r="AD220" t="inlineStr">
+        <is>
+          <t>Outside Centre</t>
+        </is>
+      </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
@@ -59094,6 +60189,11 @@
       <c r="AC221" t="n">
         <v>0</v>
       </c>
+      <c r="AD221" t="inlineStr">
+        <is>
+          <t>Number 8</t>
+        </is>
+      </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
@@ -59185,6 +60285,11 @@
       <c r="AC222" t="n">
         <v>0</v>
       </c>
+      <c r="AD222" t="inlineStr">
+        <is>
+          <t>Loose Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
@@ -59276,6 +60381,11 @@
       <c r="AC223" t="n">
         <v>0</v>
       </c>
+      <c r="AD223" t="inlineStr">
+        <is>
+          <t>Lock 5</t>
+        </is>
+      </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
@@ -59367,6 +60477,11 @@
       <c r="AC224" t="n">
         <v>0</v>
       </c>
+      <c r="AD224" t="inlineStr">
+        <is>
+          <t>Left Wing</t>
+        </is>
+      </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
@@ -59458,6 +60573,11 @@
       <c r="AC225" t="n">
         <v>0</v>
       </c>
+      <c r="AD225" t="inlineStr">
+        <is>
+          <t>Openside Flanker</t>
+        </is>
+      </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
@@ -59549,6 +60669,11 @@
       <c r="AC226" t="n">
         <v>0</v>
       </c>
+      <c r="AD226" t="inlineStr">
+        <is>
+          <t>Tight Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
@@ -59640,6 +60765,11 @@
       <c r="AC227" t="n">
         <v>0</v>
       </c>
+      <c r="AD227" t="inlineStr">
+        <is>
+          <t>Lock 4</t>
+        </is>
+      </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
@@ -59731,6 +60861,11 @@
       <c r="AC228" t="n">
         <v>0</v>
       </c>
+      <c r="AD228" t="inlineStr">
+        <is>
+          <t>Blindside Flanker</t>
+        </is>
+      </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
@@ -59822,6 +60957,11 @@
       <c r="AC229" t="n">
         <v>0</v>
       </c>
+      <c r="AD229" t="inlineStr">
+        <is>
+          <t>Fly Half</t>
+        </is>
+      </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
@@ -59913,6 +61053,11 @@
       <c r="AC230" t="n">
         <v>0</v>
       </c>
+      <c r="AD230" t="inlineStr">
+        <is>
+          <t>Loose Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
@@ -60004,6 +61149,11 @@
       <c r="AC231" t="n">
         <v>0</v>
       </c>
+      <c r="AD231" t="inlineStr">
+        <is>
+          <t>Openside Flanker</t>
+        </is>
+      </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
@@ -60095,6 +61245,11 @@
       <c r="AC232" t="n">
         <v>0</v>
       </c>
+      <c r="AD232" t="inlineStr">
+        <is>
+          <t>Loose Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
@@ -60186,6 +61341,11 @@
       <c r="AC233" t="n">
         <v>0</v>
       </c>
+      <c r="AD233" t="inlineStr">
+        <is>
+          <t>Inside Centre</t>
+        </is>
+      </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
@@ -60277,6 +61437,11 @@
       <c r="AC234" t="n">
         <v>0</v>
       </c>
+      <c r="AD234" t="inlineStr">
+        <is>
+          <t>Fullback</t>
+        </is>
+      </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
@@ -60368,6 +61533,11 @@
       <c r="AC235" t="n">
         <v>0</v>
       </c>
+      <c r="AD235" t="inlineStr">
+        <is>
+          <t>Lock 5</t>
+        </is>
+      </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
@@ -60459,6 +61629,11 @@
       <c r="AC236" t="n">
         <v>0</v>
       </c>
+      <c r="AD236" t="inlineStr">
+        <is>
+          <t>Loose Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
@@ -60550,6 +61725,11 @@
       <c r="AC237" t="n">
         <v>0</v>
       </c>
+      <c r="AD237" t="inlineStr">
+        <is>
+          <t>Openside Flanker</t>
+        </is>
+      </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
@@ -60641,6 +61821,11 @@
       <c r="AC238" t="n">
         <v>0</v>
       </c>
+      <c r="AD238" t="inlineStr">
+        <is>
+          <t>Outside Centre</t>
+        </is>
+      </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
@@ -60732,6 +61917,11 @@
       <c r="AC239" t="n">
         <v>0</v>
       </c>
+      <c r="AD239" t="inlineStr">
+        <is>
+          <t>Outside Centre</t>
+        </is>
+      </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
@@ -60823,6 +62013,11 @@
       <c r="AC240" t="n">
         <v>0</v>
       </c>
+      <c r="AD240" t="inlineStr">
+        <is>
+          <t>Fullback</t>
+        </is>
+      </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
@@ -60914,6 +62109,11 @@
       <c r="AC241" t="n">
         <v>0</v>
       </c>
+      <c r="AD241" t="inlineStr">
+        <is>
+          <t>Inside Centre</t>
+        </is>
+      </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
@@ -61005,6 +62205,11 @@
       <c r="AC242" t="n">
         <v>0</v>
       </c>
+      <c r="AD242" t="inlineStr">
+        <is>
+          <t>Openside Flanker</t>
+        </is>
+      </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
@@ -61096,6 +62301,11 @@
       <c r="AC243" t="n">
         <v>0</v>
       </c>
+      <c r="AD243" t="inlineStr">
+        <is>
+          <t>Lock 4</t>
+        </is>
+      </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
@@ -61187,6 +62397,11 @@
       <c r="AC244" t="n">
         <v>0</v>
       </c>
+      <c r="AD244" t="inlineStr">
+        <is>
+          <t>Number 8</t>
+        </is>
+      </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
@@ -61278,6 +62493,11 @@
       <c r="AC245" t="n">
         <v>0</v>
       </c>
+      <c r="AD245" t="inlineStr">
+        <is>
+          <t>Hooker</t>
+        </is>
+      </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
@@ -61369,6 +62589,11 @@
       <c r="AC246" t="n">
         <v>0</v>
       </c>
+      <c r="AD246" t="inlineStr">
+        <is>
+          <t>Lock 4</t>
+        </is>
+      </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
@@ -61460,6 +62685,11 @@
       <c r="AC247" t="n">
         <v>0</v>
       </c>
+      <c r="AD247" t="inlineStr">
+        <is>
+          <t>Lock 5</t>
+        </is>
+      </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
@@ -61551,6 +62781,11 @@
       <c r="AC248" t="n">
         <v>0</v>
       </c>
+      <c r="AD248" t="inlineStr">
+        <is>
+          <t>Openside Flanker</t>
+        </is>
+      </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
@@ -61642,6 +62877,11 @@
       <c r="AC249" t="n">
         <v>0</v>
       </c>
+      <c r="AD249" t="inlineStr">
+        <is>
+          <t>Number 8</t>
+        </is>
+      </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
@@ -61733,6 +62973,11 @@
       <c r="AC250" t="n">
         <v>0</v>
       </c>
+      <c r="AD250" t="inlineStr">
+        <is>
+          <t>Openside Flanker</t>
+        </is>
+      </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
@@ -61824,6 +63069,11 @@
       <c r="AC251" t="n">
         <v>0</v>
       </c>
+      <c r="AD251" t="inlineStr">
+        <is>
+          <t>Fly Half</t>
+        </is>
+      </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
@@ -61915,6 +63165,11 @@
       <c r="AC252" t="n">
         <v>0</v>
       </c>
+      <c r="AD252" t="inlineStr">
+        <is>
+          <t>Lock 5</t>
+        </is>
+      </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
@@ -62006,6 +63261,11 @@
       <c r="AC253" t="n">
         <v>0</v>
       </c>
+      <c r="AD253" t="inlineStr">
+        <is>
+          <t>Blindside Flanker</t>
+        </is>
+      </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
@@ -62097,6 +63357,11 @@
       <c r="AC254" t="n">
         <v>0</v>
       </c>
+      <c r="AD254" t="inlineStr">
+        <is>
+          <t>Number 8</t>
+        </is>
+      </c>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
@@ -62188,6 +63453,11 @@
       <c r="AC255" t="n">
         <v>0</v>
       </c>
+      <c r="AD255" t="inlineStr">
+        <is>
+          <t>Fly Half</t>
+        </is>
+      </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
@@ -62279,6 +63549,11 @@
       <c r="AC256" t="n">
         <v>0</v>
       </c>
+      <c r="AD256" t="inlineStr">
+        <is>
+          <t>Loose Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
@@ -62370,6 +63645,11 @@
       <c r="AC257" t="n">
         <v>0</v>
       </c>
+      <c r="AD257" t="inlineStr">
+        <is>
+          <t>Inside Centre</t>
+        </is>
+      </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
@@ -62461,6 +63741,11 @@
       <c r="AC258" t="n">
         <v>0</v>
       </c>
+      <c r="AD258" t="inlineStr">
+        <is>
+          <t>Loose Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
@@ -62552,6 +63837,11 @@
       <c r="AC259" t="n">
         <v>0</v>
       </c>
+      <c r="AD259" t="inlineStr">
+        <is>
+          <t>Inside Centre</t>
+        </is>
+      </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
@@ -62643,6 +63933,11 @@
       <c r="AC260" t="n">
         <v>0</v>
       </c>
+      <c r="AD260" t="inlineStr">
+        <is>
+          <t>Hooker</t>
+        </is>
+      </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
@@ -62734,6 +64029,11 @@
       <c r="AC261" t="n">
         <v>0</v>
       </c>
+      <c r="AD261" t="inlineStr">
+        <is>
+          <t>Lock 5</t>
+        </is>
+      </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
@@ -62825,6 +64125,11 @@
       <c r="AC262" t="n">
         <v>0</v>
       </c>
+      <c r="AD262" t="inlineStr">
+        <is>
+          <t>Left Wing</t>
+        </is>
+      </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
@@ -62916,6 +64221,11 @@
       <c r="AC263" t="n">
         <v>0</v>
       </c>
+      <c r="AD263" t="inlineStr">
+        <is>
+          <t>Hooker</t>
+        </is>
+      </c>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
@@ -63007,6 +64317,11 @@
       <c r="AC264" t="n">
         <v>0</v>
       </c>
+      <c r="AD264" t="inlineStr">
+        <is>
+          <t>Lock 5</t>
+        </is>
+      </c>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
@@ -63098,6 +64413,11 @@
       <c r="AC265" t="n">
         <v>0</v>
       </c>
+      <c r="AD265" t="inlineStr">
+        <is>
+          <t>Loose Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
@@ -63189,6 +64509,11 @@
       <c r="AC266" t="n">
         <v>0</v>
       </c>
+      <c r="AD266" t="inlineStr">
+        <is>
+          <t>Scrum Half</t>
+        </is>
+      </c>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
@@ -63280,6 +64605,11 @@
       <c r="AC267" t="n">
         <v>0</v>
       </c>
+      <c r="AD267" t="inlineStr">
+        <is>
+          <t>Fly Half</t>
+        </is>
+      </c>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
@@ -63371,6 +64701,11 @@
       <c r="AC268" t="n">
         <v>0</v>
       </c>
+      <c r="AD268" t="inlineStr">
+        <is>
+          <t>Outside Centre</t>
+        </is>
+      </c>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
@@ -63462,6 +64797,11 @@
       <c r="AC269" t="n">
         <v>0</v>
       </c>
+      <c r="AD269" t="inlineStr">
+        <is>
+          <t>Scrum Half</t>
+        </is>
+      </c>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
@@ -63553,6 +64893,11 @@
       <c r="AC270" t="n">
         <v>0</v>
       </c>
+      <c r="AD270" t="inlineStr">
+        <is>
+          <t>Inside Centre</t>
+        </is>
+      </c>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
@@ -63644,6 +64989,11 @@
       <c r="AC271" t="n">
         <v>0</v>
       </c>
+      <c r="AD271" t="inlineStr">
+        <is>
+          <t>Fly Half</t>
+        </is>
+      </c>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
@@ -63735,6 +65085,11 @@
       <c r="AC272" t="n">
         <v>0</v>
       </c>
+      <c r="AD272" t="inlineStr">
+        <is>
+          <t>Fly Half</t>
+        </is>
+      </c>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
@@ -63826,6 +65181,11 @@
       <c r="AC273" t="n">
         <v>0</v>
       </c>
+      <c r="AD273" t="inlineStr">
+        <is>
+          <t>Tight Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
@@ -63917,6 +65277,11 @@
       <c r="AC274" t="n">
         <v>0</v>
       </c>
+      <c r="AD274" t="inlineStr">
+        <is>
+          <t>Right Wing</t>
+        </is>
+      </c>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
@@ -64008,6 +65373,11 @@
       <c r="AC275" t="n">
         <v>0</v>
       </c>
+      <c r="AD275" t="inlineStr">
+        <is>
+          <t>Blindside Flanker</t>
+        </is>
+      </c>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
@@ -64099,6 +65469,11 @@
       <c r="AC276" t="n">
         <v>0</v>
       </c>
+      <c r="AD276" t="inlineStr">
+        <is>
+          <t>Lock 4</t>
+        </is>
+      </c>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
@@ -64190,6 +65565,11 @@
       <c r="AC277" t="n">
         <v>0</v>
       </c>
+      <c r="AD277" t="inlineStr">
+        <is>
+          <t>Loose Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="278">
       <c r="A278" t="inlineStr">
@@ -64281,6 +65661,11 @@
       <c r="AC278" t="n">
         <v>0</v>
       </c>
+      <c r="AD278" t="inlineStr">
+        <is>
+          <t>Inside Centre</t>
+        </is>
+      </c>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
@@ -64372,6 +65757,11 @@
       <c r="AC279" t="n">
         <v>0</v>
       </c>
+      <c r="AD279" t="inlineStr">
+        <is>
+          <t>Scrum Half</t>
+        </is>
+      </c>
     </row>
     <row r="280">
       <c r="A280" t="inlineStr">
@@ -64463,6 +65853,11 @@
       <c r="AC280" t="n">
         <v>0</v>
       </c>
+      <c r="AD280" t="inlineStr">
+        <is>
+          <t>Left Wing</t>
+        </is>
+      </c>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
@@ -64554,6 +65949,11 @@
       <c r="AC281" t="n">
         <v>0</v>
       </c>
+      <c r="AD281" t="inlineStr">
+        <is>
+          <t>Fly Half</t>
+        </is>
+      </c>
     </row>
     <row r="282">
       <c r="A282" t="inlineStr">
@@ -64645,6 +66045,11 @@
       <c r="AC282" t="n">
         <v>0</v>
       </c>
+      <c r="AD282" t="inlineStr">
+        <is>
+          <t>Outside Centre</t>
+        </is>
+      </c>
     </row>
     <row r="283">
       <c r="A283" t="inlineStr">
@@ -64736,6 +66141,11 @@
       <c r="AC283" t="n">
         <v>0</v>
       </c>
+      <c r="AD283" t="inlineStr">
+        <is>
+          <t>Scrum Half</t>
+        </is>
+      </c>
     </row>
     <row r="284">
       <c r="A284" t="inlineStr">
@@ -64827,6 +66237,11 @@
       <c r="AC284" t="n">
         <v>0</v>
       </c>
+      <c r="AD284" t="inlineStr">
+        <is>
+          <t>Left Wing</t>
+        </is>
+      </c>
     </row>
     <row r="285">
       <c r="A285" t="inlineStr">
@@ -64918,6 +66333,11 @@
       <c r="AC285" t="n">
         <v>0</v>
       </c>
+      <c r="AD285" t="inlineStr">
+        <is>
+          <t>Fullback</t>
+        </is>
+      </c>
     </row>
     <row r="286">
       <c r="A286" t="inlineStr">
@@ -65009,6 +66429,11 @@
       <c r="AC286" t="n">
         <v>0</v>
       </c>
+      <c r="AD286" t="inlineStr">
+        <is>
+          <t>Number 8</t>
+        </is>
+      </c>
     </row>
     <row r="287">
       <c r="A287" t="inlineStr">
@@ -65100,6 +66525,11 @@
       <c r="AC287" t="n">
         <v>0</v>
       </c>
+      <c r="AD287" t="inlineStr">
+        <is>
+          <t>Right Wing</t>
+        </is>
+      </c>
     </row>
     <row r="288">
       <c r="A288" t="inlineStr">
@@ -65191,6 +66621,11 @@
       <c r="AC288" t="n">
         <v>0</v>
       </c>
+      <c r="AD288" t="inlineStr">
+        <is>
+          <t>Fly Half</t>
+        </is>
+      </c>
     </row>
     <row r="289">
       <c r="A289" t="inlineStr">
@@ -65282,6 +66717,11 @@
       <c r="AC289" t="n">
         <v>0</v>
       </c>
+      <c r="AD289" t="inlineStr">
+        <is>
+          <t>Hooker</t>
+        </is>
+      </c>
     </row>
     <row r="290">
       <c r="A290" t="inlineStr">
@@ -65373,6 +66813,11 @@
       <c r="AC290" t="n">
         <v>0</v>
       </c>
+      <c r="AD290" t="inlineStr">
+        <is>
+          <t>Fly Half</t>
+        </is>
+      </c>
     </row>
     <row r="291">
       <c r="A291" t="inlineStr">
@@ -65464,6 +66909,11 @@
       <c r="AC291" t="n">
         <v>0</v>
       </c>
+      <c r="AD291" t="inlineStr">
+        <is>
+          <t>Hooker</t>
+        </is>
+      </c>
     </row>
     <row r="292">
       <c r="A292" t="inlineStr">
@@ -65555,6 +67005,11 @@
       <c r="AC292" t="n">
         <v>0</v>
       </c>
+      <c r="AD292" t="inlineStr">
+        <is>
+          <t>Tight Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="293">
       <c r="A293" t="inlineStr">
@@ -65646,6 +67101,11 @@
       <c r="AC293" t="n">
         <v>0</v>
       </c>
+      <c r="AD293" t="inlineStr">
+        <is>
+          <t>Scrum Half</t>
+        </is>
+      </c>
     </row>
     <row r="294">
       <c r="A294" t="inlineStr">
@@ -65737,6 +67197,11 @@
       <c r="AC294" t="n">
         <v>0</v>
       </c>
+      <c r="AD294" t="inlineStr">
+        <is>
+          <t>Openside Flanker</t>
+        </is>
+      </c>
     </row>
     <row r="295">
       <c r="A295" t="inlineStr">
@@ -65828,6 +67293,11 @@
       <c r="AC295" t="n">
         <v>0</v>
       </c>
+      <c r="AD295" t="inlineStr">
+        <is>
+          <t>Outside Centre</t>
+        </is>
+      </c>
     </row>
     <row r="296">
       <c r="A296" t="inlineStr">
@@ -65919,6 +67389,11 @@
       <c r="AC296" t="n">
         <v>0</v>
       </c>
+      <c r="AD296" t="inlineStr">
+        <is>
+          <t>Left Wing</t>
+        </is>
+      </c>
     </row>
     <row r="297">
       <c r="A297" t="inlineStr">
@@ -66010,6 +67485,11 @@
       <c r="AC297" t="n">
         <v>0</v>
       </c>
+      <c r="AD297" t="inlineStr">
+        <is>
+          <t>Blindside Flanker</t>
+        </is>
+      </c>
     </row>
     <row r="298">
       <c r="A298" t="inlineStr">
@@ -66101,6 +67581,11 @@
       <c r="AC298" t="n">
         <v>0</v>
       </c>
+      <c r="AD298" t="inlineStr">
+        <is>
+          <t>Scrum Half</t>
+        </is>
+      </c>
     </row>
     <row r="299">
       <c r="A299" t="inlineStr">
@@ -66192,6 +67677,11 @@
       <c r="AC299" t="n">
         <v>0</v>
       </c>
+      <c r="AD299" t="inlineStr">
+        <is>
+          <t>Hooker</t>
+        </is>
+      </c>
     </row>
     <row r="300">
       <c r="A300" t="inlineStr">
@@ -66283,6 +67773,11 @@
       <c r="AC300" t="n">
         <v>0</v>
       </c>
+      <c r="AD300" t="inlineStr">
+        <is>
+          <t>Scrum Half</t>
+        </is>
+      </c>
     </row>
     <row r="301">
       <c r="A301" t="inlineStr">
@@ -66374,6 +67869,11 @@
       <c r="AC301" t="n">
         <v>0</v>
       </c>
+      <c r="AD301" t="inlineStr">
+        <is>
+          <t>Outside Centre</t>
+        </is>
+      </c>
     </row>
     <row r="302">
       <c r="A302" t="inlineStr">
@@ -66465,6 +67965,11 @@
       <c r="AC302" t="n">
         <v>0</v>
       </c>
+      <c r="AD302" t="inlineStr">
+        <is>
+          <t>Fullback</t>
+        </is>
+      </c>
     </row>
     <row r="303">
       <c r="A303" t="inlineStr">
@@ -66556,6 +68061,11 @@
       <c r="AC303" t="n">
         <v>0</v>
       </c>
+      <c r="AD303" t="inlineStr">
+        <is>
+          <t>Number 8</t>
+        </is>
+      </c>
     </row>
     <row r="304">
       <c r="A304" t="inlineStr">
@@ -66647,6 +68157,11 @@
       <c r="AC304" t="n">
         <v>0</v>
       </c>
+      <c r="AD304" t="inlineStr">
+        <is>
+          <t>Loose Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="305">
       <c r="A305" t="inlineStr">
@@ -66738,6 +68253,11 @@
       <c r="AC305" t="n">
         <v>0</v>
       </c>
+      <c r="AD305" t="inlineStr">
+        <is>
+          <t>Lock 5</t>
+        </is>
+      </c>
     </row>
     <row r="306">
       <c r="A306" t="inlineStr">
@@ -66829,6 +68349,11 @@
       <c r="AC306" t="n">
         <v>0</v>
       </c>
+      <c r="AD306" t="inlineStr">
+        <is>
+          <t>Fullback</t>
+        </is>
+      </c>
     </row>
     <row r="307">
       <c r="A307" t="inlineStr">
@@ -66920,6 +68445,11 @@
       <c r="AC307" t="n">
         <v>0</v>
       </c>
+      <c r="AD307" t="inlineStr">
+        <is>
+          <t>Openside Flanker</t>
+        </is>
+      </c>
     </row>
     <row r="308">
       <c r="A308" t="inlineStr">
@@ -67011,6 +68541,11 @@
       <c r="AC308" t="n">
         <v>0</v>
       </c>
+      <c r="AD308" t="inlineStr">
+        <is>
+          <t>Blindside Flanker</t>
+        </is>
+      </c>
     </row>
     <row r="309">
       <c r="A309" t="inlineStr">
@@ -67102,6 +68637,11 @@
       <c r="AC309" t="n">
         <v>0</v>
       </c>
+      <c r="AD309" t="inlineStr">
+        <is>
+          <t>Tight Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="310">
       <c r="A310" t="inlineStr">
@@ -67193,6 +68733,11 @@
       <c r="AC310" t="n">
         <v>0</v>
       </c>
+      <c r="AD310" t="inlineStr">
+        <is>
+          <t>Hooker</t>
+        </is>
+      </c>
     </row>
     <row r="311">
       <c r="A311" t="inlineStr">
@@ -67284,6 +68829,11 @@
       <c r="AC311" t="n">
         <v>0</v>
       </c>
+      <c r="AD311" t="inlineStr">
+        <is>
+          <t>Hooker</t>
+        </is>
+      </c>
     </row>
     <row r="312">
       <c r="A312" t="inlineStr">
@@ -67375,6 +68925,11 @@
       <c r="AC312" t="n">
         <v>0</v>
       </c>
+      <c r="AD312" t="inlineStr">
+        <is>
+          <t>Hooker</t>
+        </is>
+      </c>
     </row>
     <row r="313">
       <c r="A313" t="inlineStr">
@@ -67466,6 +69021,11 @@
       <c r="AC313" t="n">
         <v>0</v>
       </c>
+      <c r="AD313" t="inlineStr">
+        <is>
+          <t>Lock 5</t>
+        </is>
+      </c>
     </row>
     <row r="314">
       <c r="A314" t="inlineStr">
@@ -67557,6 +69117,11 @@
       <c r="AC314" t="n">
         <v>0</v>
       </c>
+      <c r="AD314" t="inlineStr">
+        <is>
+          <t>Blindside Flanker</t>
+        </is>
+      </c>
     </row>
     <row r="315">
       <c r="A315" t="inlineStr">
@@ -67648,6 +69213,11 @@
       <c r="AC315" t="n">
         <v>0</v>
       </c>
+      <c r="AD315" t="inlineStr">
+        <is>
+          <t>Tight Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="316">
       <c r="A316" t="inlineStr">
@@ -67739,6 +69309,11 @@
       <c r="AC316" t="n">
         <v>0</v>
       </c>
+      <c r="AD316" t="inlineStr">
+        <is>
+          <t>Left Wing</t>
+        </is>
+      </c>
     </row>
     <row r="317">
       <c r="A317" t="inlineStr">
@@ -67830,6 +69405,11 @@
       <c r="AC317" t="n">
         <v>0</v>
       </c>
+      <c r="AD317" t="inlineStr">
+        <is>
+          <t>Left Wing</t>
+        </is>
+      </c>
     </row>
     <row r="318">
       <c r="A318" t="inlineStr">
@@ -67921,6 +69501,11 @@
       <c r="AC318" t="n">
         <v>0</v>
       </c>
+      <c r="AD318" t="inlineStr">
+        <is>
+          <t>Openside Flanker</t>
+        </is>
+      </c>
     </row>
     <row r="319">
       <c r="A319" t="inlineStr">
@@ -68012,6 +69597,11 @@
       <c r="AC319" t="n">
         <v>0</v>
       </c>
+      <c r="AD319" t="inlineStr">
+        <is>
+          <t>Lock 5</t>
+        </is>
+      </c>
     </row>
     <row r="320">
       <c r="A320" t="inlineStr">
@@ -68103,6 +69693,11 @@
       <c r="AC320" t="n">
         <v>0</v>
       </c>
+      <c r="AD320" t="inlineStr">
+        <is>
+          <t>Scrum Half</t>
+        </is>
+      </c>
     </row>
     <row r="321">
       <c r="A321" t="inlineStr">
@@ -68194,6 +69789,11 @@
       <c r="AC321" t="n">
         <v>0</v>
       </c>
+      <c r="AD321" t="inlineStr">
+        <is>
+          <t>Outside Centre</t>
+        </is>
+      </c>
     </row>
     <row r="322">
       <c r="A322" t="inlineStr">
@@ -68285,6 +69885,11 @@
       <c r="AC322" t="n">
         <v>0</v>
       </c>
+      <c r="AD322" t="inlineStr">
+        <is>
+          <t>Right Wing</t>
+        </is>
+      </c>
     </row>
     <row r="323">
       <c r="A323" t="inlineStr">
@@ -68376,6 +69981,11 @@
       <c r="AC323" t="n">
         <v>1</v>
       </c>
+      <c r="AD323" t="inlineStr">
+        <is>
+          <t>Fly Half</t>
+        </is>
+      </c>
     </row>
     <row r="324">
       <c r="A324" t="inlineStr">
@@ -68467,6 +70077,11 @@
       <c r="AC324" t="n">
         <v>0</v>
       </c>
+      <c r="AD324" t="inlineStr">
+        <is>
+          <t>Left Wing</t>
+        </is>
+      </c>
     </row>
     <row r="325">
       <c r="A325" t="inlineStr">
@@ -68558,6 +70173,11 @@
       <c r="AC325" t="n">
         <v>0</v>
       </c>
+      <c r="AD325" t="inlineStr">
+        <is>
+          <t>Lock 4</t>
+        </is>
+      </c>
     </row>
     <row r="326">
       <c r="A326" t="inlineStr">
@@ -68649,6 +70269,11 @@
       <c r="AC326" t="n">
         <v>0</v>
       </c>
+      <c r="AD326" t="inlineStr">
+        <is>
+          <t>Tight Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="327">
       <c r="A327" t="inlineStr">
@@ -68740,6 +70365,11 @@
       <c r="AC327" t="n">
         <v>0</v>
       </c>
+      <c r="AD327" t="inlineStr">
+        <is>
+          <t>Left Wing</t>
+        </is>
+      </c>
     </row>
     <row r="328">
       <c r="A328" t="inlineStr">
@@ -68831,6 +70461,11 @@
       <c r="AC328" t="n">
         <v>0</v>
       </c>
+      <c r="AD328" t="inlineStr">
+        <is>
+          <t>Lock 4</t>
+        </is>
+      </c>
     </row>
     <row r="329">
       <c r="A329" t="inlineStr">
@@ -68922,6 +70557,11 @@
       <c r="AC329" t="n">
         <v>1</v>
       </c>
+      <c r="AD329" t="inlineStr">
+        <is>
+          <t>Lock 5</t>
+        </is>
+      </c>
     </row>
     <row r="330">
       <c r="A330" t="inlineStr">
@@ -69013,6 +70653,11 @@
       <c r="AC330" t="n">
         <v>0</v>
       </c>
+      <c r="AD330" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="331">
       <c r="A331" t="inlineStr">
@@ -69104,6 +70749,11 @@
       <c r="AC331" t="n">
         <v>0</v>
       </c>
+      <c r="AD331" t="inlineStr">
+        <is>
+          <t>Loose Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="332">
       <c r="A332" t="inlineStr">
@@ -69195,6 +70845,11 @@
       <c r="AC332" t="n">
         <v>0</v>
       </c>
+      <c r="AD332" t="inlineStr">
+        <is>
+          <t>Openside Flanker</t>
+        </is>
+      </c>
     </row>
     <row r="333">
       <c r="A333" t="inlineStr">
@@ -69286,6 +70941,11 @@
       <c r="AC333" t="n">
         <v>0</v>
       </c>
+      <c r="AD333" t="inlineStr">
+        <is>
+          <t>Openside Flanker</t>
+        </is>
+      </c>
     </row>
     <row r="334">
       <c r="A334" t="inlineStr">
@@ -69377,6 +71037,11 @@
       <c r="AC334" t="n">
         <v>0</v>
       </c>
+      <c r="AD334" t="inlineStr">
+        <is>
+          <t>Blindside Flanker</t>
+        </is>
+      </c>
     </row>
     <row r="335">
       <c r="A335" t="inlineStr">
@@ -69468,6 +71133,11 @@
       <c r="AC335" t="n">
         <v>0</v>
       </c>
+      <c r="AD335" t="inlineStr">
+        <is>
+          <t>Loose Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="336">
       <c r="A336" t="inlineStr">
@@ -69559,6 +71229,11 @@
       <c r="AC336" t="n">
         <v>0</v>
       </c>
+      <c r="AD336" t="inlineStr">
+        <is>
+          <t>Loose Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="337">
       <c r="A337" t="inlineStr">
@@ -69650,6 +71325,11 @@
       <c r="AC337" t="n">
         <v>0</v>
       </c>
+      <c r="AD337" t="inlineStr">
+        <is>
+          <t>Loose Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="338">
       <c r="A338" t="inlineStr">
@@ -69741,6 +71421,11 @@
       <c r="AC338" t="n">
         <v>0</v>
       </c>
+      <c r="AD338" t="inlineStr">
+        <is>
+          <t>Tight Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="339">
       <c r="A339" t="inlineStr">
@@ -69832,6 +71517,11 @@
       <c r="AC339" t="n">
         <v>0</v>
       </c>
+      <c r="AD339" t="inlineStr">
+        <is>
+          <t>Loose Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="340">
       <c r="A340" t="inlineStr">
@@ -69923,6 +71613,11 @@
       <c r="AC340" t="n">
         <v>1</v>
       </c>
+      <c r="AD340" t="inlineStr">
+        <is>
+          <t>Inside Centre</t>
+        </is>
+      </c>
     </row>
     <row r="341">
       <c r="A341" t="inlineStr">
@@ -70014,6 +71709,11 @@
       <c r="AC341" t="n">
         <v>0</v>
       </c>
+      <c r="AD341" t="inlineStr">
+        <is>
+          <t>Inside Centre</t>
+        </is>
+      </c>
     </row>
     <row r="342">
       <c r="A342" t="inlineStr">
@@ -70105,6 +71805,11 @@
       <c r="AC342" t="n">
         <v>0</v>
       </c>
+      <c r="AD342" t="inlineStr">
+        <is>
+          <t>Lock 5</t>
+        </is>
+      </c>
     </row>
     <row r="343">
       <c r="A343" t="inlineStr">
@@ -70196,6 +71901,11 @@
       <c r="AC343" t="n">
         <v>0</v>
       </c>
+      <c r="AD343" t="inlineStr">
+        <is>
+          <t>Tight Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="344">
       <c r="A344" t="inlineStr">
@@ -70287,6 +71997,11 @@
       <c r="AC344" t="n">
         <v>0</v>
       </c>
+      <c r="AD344" t="inlineStr">
+        <is>
+          <t>Fly Half</t>
+        </is>
+      </c>
     </row>
     <row r="345">
       <c r="A345" t="inlineStr">
@@ -70378,6 +72093,11 @@
       <c r="AC345" t="n">
         <v>0</v>
       </c>
+      <c r="AD345" t="inlineStr">
+        <is>
+          <t>Number 8</t>
+        </is>
+      </c>
     </row>
     <row r="346">
       <c r="A346" t="inlineStr">
@@ -70469,6 +72189,11 @@
       <c r="AC346" t="n">
         <v>0</v>
       </c>
+      <c r="AD346" t="inlineStr">
+        <is>
+          <t>Lock 5</t>
+        </is>
+      </c>
     </row>
     <row r="347">
       <c r="A347" t="inlineStr">
@@ -70560,6 +72285,11 @@
       <c r="AC347" t="n">
         <v>1</v>
       </c>
+      <c r="AD347" t="inlineStr">
+        <is>
+          <t>Tight Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="348">
       <c r="A348" t="inlineStr">
@@ -70651,6 +72381,11 @@
       <c r="AC348" t="n">
         <v>0</v>
       </c>
+      <c r="AD348" t="inlineStr">
+        <is>
+          <t>Lock 4</t>
+        </is>
+      </c>
     </row>
     <row r="349">
       <c r="A349" t="inlineStr">
@@ -70742,6 +72477,11 @@
       <c r="AC349" t="n">
         <v>0</v>
       </c>
+      <c r="AD349" t="inlineStr">
+        <is>
+          <t>Fly Half</t>
+        </is>
+      </c>
     </row>
     <row r="350">
       <c r="A350" t="inlineStr">
@@ -70833,6 +72573,11 @@
       <c r="AC350" t="n">
         <v>0</v>
       </c>
+      <c r="AD350" t="inlineStr">
+        <is>
+          <t>Lock 5</t>
+        </is>
+      </c>
     </row>
     <row r="351">
       <c r="A351" t="inlineStr">
@@ -70924,6 +72669,11 @@
       <c r="AC351" t="n">
         <v>0</v>
       </c>
+      <c r="AD351" t="inlineStr">
+        <is>
+          <t>Hooker</t>
+        </is>
+      </c>
     </row>
     <row r="352">
       <c r="A352" t="inlineStr">
@@ -71015,6 +72765,11 @@
       <c r="AC352" t="n">
         <v>1</v>
       </c>
+      <c r="AD352" t="inlineStr">
+        <is>
+          <t>Openside Flanker</t>
+        </is>
+      </c>
     </row>
     <row r="353">
       <c r="A353" t="inlineStr">
@@ -71106,6 +72861,11 @@
       <c r="AC353" t="n">
         <v>0</v>
       </c>
+      <c r="AD353" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="354">
       <c r="A354" t="inlineStr">
@@ -71197,6 +72957,11 @@
       <c r="AC354" t="n">
         <v>0</v>
       </c>
+      <c r="AD354" t="inlineStr">
+        <is>
+          <t>Outside Centre</t>
+        </is>
+      </c>
     </row>
     <row r="355">
       <c r="A355" t="inlineStr">
@@ -71288,6 +73053,11 @@
       <c r="AC355" t="n">
         <v>0</v>
       </c>
+      <c r="AD355" t="inlineStr">
+        <is>
+          <t>Outside Centre</t>
+        </is>
+      </c>
     </row>
     <row r="356">
       <c r="A356" t="inlineStr">
@@ -71379,6 +73149,11 @@
       <c r="AC356" t="n">
         <v>0</v>
       </c>
+      <c r="AD356" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="357">
       <c r="A357" t="inlineStr">
@@ -71470,6 +73245,11 @@
       <c r="AC357" t="n">
         <v>0</v>
       </c>
+      <c r="AD357" t="inlineStr">
+        <is>
+          <t>Inside Centre</t>
+        </is>
+      </c>
     </row>
     <row r="358">
       <c r="A358" t="inlineStr">
@@ -71561,6 +73341,11 @@
       <c r="AC358" t="n">
         <v>0</v>
       </c>
+      <c r="AD358" t="inlineStr">
+        <is>
+          <t>Openside Flanker</t>
+        </is>
+      </c>
     </row>
     <row r="359">
       <c r="A359" t="inlineStr">
@@ -71652,6 +73437,11 @@
       <c r="AC359" t="n">
         <v>0</v>
       </c>
+      <c r="AD359" t="inlineStr">
+        <is>
+          <t>Lock 4</t>
+        </is>
+      </c>
     </row>
     <row r="360">
       <c r="A360" t="inlineStr">
@@ -71743,6 +73533,11 @@
       <c r="AC360" t="n">
         <v>0</v>
       </c>
+      <c r="AD360" t="inlineStr">
+        <is>
+          <t>Number 8</t>
+        </is>
+      </c>
     </row>
     <row r="361">
       <c r="A361" t="inlineStr">
@@ -71834,6 +73629,11 @@
       <c r="AC361" t="n">
         <v>0</v>
       </c>
+      <c r="AD361" t="inlineStr">
+        <is>
+          <t>Lock 4</t>
+        </is>
+      </c>
     </row>
     <row r="362">
       <c r="A362" t="inlineStr">
@@ -71925,6 +73725,11 @@
       <c r="AC362" t="n">
         <v>0</v>
       </c>
+      <c r="AD362" t="inlineStr">
+        <is>
+          <t>Lock 5</t>
+        </is>
+      </c>
     </row>
     <row r="363">
       <c r="A363" t="inlineStr">
@@ -72016,6 +73821,11 @@
       <c r="AC363" t="n">
         <v>0</v>
       </c>
+      <c r="AD363" t="inlineStr">
+        <is>
+          <t>Openside Flanker</t>
+        </is>
+      </c>
     </row>
     <row r="364">
       <c r="A364" t="inlineStr">
@@ -72107,6 +73917,11 @@
       <c r="AC364" t="n">
         <v>0</v>
       </c>
+      <c r="AD364" t="inlineStr">
+        <is>
+          <t>Number 8</t>
+        </is>
+      </c>
     </row>
     <row r="365">
       <c r="A365" t="inlineStr">
@@ -72198,6 +74013,11 @@
       <c r="AC365" t="n">
         <v>0</v>
       </c>
+      <c r="AD365" t="inlineStr">
+        <is>
+          <t>Openside Flanker</t>
+        </is>
+      </c>
     </row>
     <row r="366">
       <c r="A366" t="inlineStr">
@@ -72289,6 +74109,11 @@
       <c r="AC366" t="n">
         <v>0</v>
       </c>
+      <c r="AD366" t="inlineStr">
+        <is>
+          <t>Fly Half</t>
+        </is>
+      </c>
     </row>
     <row r="367">
       <c r="A367" t="inlineStr">
@@ -72380,6 +74205,11 @@
       <c r="AC367" t="n">
         <v>0</v>
       </c>
+      <c r="AD367" t="inlineStr">
+        <is>
+          <t>Loose Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="368">
       <c r="A368" t="inlineStr">
@@ -72471,6 +74301,11 @@
       <c r="AC368" t="n">
         <v>0</v>
       </c>
+      <c r="AD368" t="inlineStr">
+        <is>
+          <t>Tight Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="369">
       <c r="A369" t="inlineStr">
@@ -72562,6 +74397,11 @@
       <c r="AC369" t="n">
         <v>0</v>
       </c>
+      <c r="AD369" t="inlineStr">
+        <is>
+          <t>Loose Head Prop</t>
+        </is>
+      </c>
     </row>
     <row r="370">
       <c r="A370" t="inlineStr">
@@ -72652,6 +74492,11 @@
       </c>
       <c r="AC370" t="n">
         <v>0</v>
+      </c>
+      <c r="AD370" t="inlineStr">
+        <is>
+          <t>Hooker</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>